<commit_message>
Venta, Guion y mejora de estetica en taller
</commit_message>
<xml_diff>
--- a/Actividades/Taller02011/Caminos.xlsx
+++ b/Actividades/Taller02011/Caminos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Downloads\Taller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\ProyectoFinal2019-\Actividades\Taller02011\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BA9B3E-853A-474C-9491-B6E9AEBE6990}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A201C1C-219F-44C6-B57E-6DC471845645}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{AE4EEE34-6B0C-4C70-869A-1F1E2D9FD606}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AE4EEE34-6B0C-4C70-869A-1F1E2D9FD606}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -608,7 +608,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -634,8 +634,46 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="22"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF0070C0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -644,48 +682,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -752,58 +760,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -812,6 +796,59 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1183,24 +1220,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC705236-79BB-4129-AE87-577426D2C43E}">
-  <dimension ref="A1:O94"/>
+  <dimension ref="A1:O95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.85546875" customWidth="1"/>
-    <col min="6" max="6" width="38.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.42578125" customWidth="1"/>
-    <col min="10" max="10" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" customWidth="1"/>
     <col min="11" max="11" width="39.140625" customWidth="1"/>
     <col min="12" max="12" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
@@ -1208,878 +1245,871 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:15" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="4" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="5" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="H4" s="17" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-    </row>
-    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:15" ht="25.5" x14ac:dyDescent="0.5">
+      <c r="A6" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D6" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E6" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G6" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-    </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+    </row>
+    <row r="7" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B7" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C7" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D7" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E7" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="G6" s="19"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="F7" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B8" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C8" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D8" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E8" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="F8" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B9" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C9" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D9" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E9" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="F9" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B10" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C10" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D10" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E10" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="F10" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B11" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C11" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D11" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E11" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="F11" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B12" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C12" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D12" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E12" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="F12" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B13" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C13" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D13" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E13" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="F13" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B14" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C14" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D14" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E14" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="F14" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B15" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C15" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D15" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E15" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="F15" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B16" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C16" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D16" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E16" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="F16" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B17" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C17" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D17" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E17" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="F16" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="F17" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B18" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C18" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D18" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E18" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="F17" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="F18" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B19" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C19" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D19" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E19" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="F19" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B20" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C20" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D20" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E20" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="F20" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B21" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C21" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D21" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E21" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="F21" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B22" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C22" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D22" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E22" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="F21" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="F22" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B23" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C23" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D23" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E23" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="F22" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="F23" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B24" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C24" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D24" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E24" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="F23" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="F24" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B25" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C25" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D25" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E25" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="F24" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="F25" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B26" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C26" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D26" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E26" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="F25" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="F26" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A27" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B27" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C27" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D27" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E27" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F26" s="10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="F27" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A28" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B28" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C28" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D28" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E28" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F27" s="10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="F28" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B29" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C29" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D29" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E29" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F28" s="10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="F29" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A30" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B30" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C30" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D30" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E30" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F29" s="10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="F30" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A31" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B31" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C31" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D31" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E31" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F30" s="10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="F31" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B32" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C32" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D32" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E32" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F31" s="10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+      <c r="F32" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A33" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B33" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C33" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D33" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E33" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F32" s="10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+      <c r="F33" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A34" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B34" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C34" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D34" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E34" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F33" s="10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+      <c r="F34" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A35" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B35" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C35" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D35" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E35" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F34" s="10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+      <c r="F35" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A36" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B36" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C36" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D36" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E36" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F35" s="10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+      <c r="F36" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A37" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B37" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C37" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D37" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E37" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F36" s="10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+      <c r="F37" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A38" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B38" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C38" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D38" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E38" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="F37" s="10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+      <c r="F38" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A39" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B39" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C39" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D39" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E39" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F39" s="24" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+    <row r="40" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A40" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B40" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C40" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D40" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E40" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="F40" s="24" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
+    <row r="41" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A41" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B41" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C41" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D41" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E41" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F41" s="24" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
+    <row r="42" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A42" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B42" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C42" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D42" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E42" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F42" s="24" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A44" s="15" t="s">
+    <row r="45" spans="1:8" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="A45" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="15"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="25"/>
+    </row>
+    <row r="46" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A46" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B46" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C46" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D46" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E46" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="G45" s="3" t="s">
+      <c r="F46" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="G46" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="H45" s="3" t="s">
+      <c r="H46" s="11" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F46" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="G46" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H46" s="12" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E47" s="12" t="s">
         <v>178</v>
@@ -2096,22 +2126,22 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E48" s="12" t="s">
         <v>178</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G48" s="12" t="s">
         <v>20</v>
@@ -2122,22 +2152,22 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C49" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E49" s="12" t="s">
         <v>178</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G49" s="12" t="s">
         <v>20</v>
@@ -2147,995 +2177,1028 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B51" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C50" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D50" s="11" t="s">
+      <c r="C51" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="E51" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F50" s="11" t="s">
+      <c r="F51" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="G50" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H50" s="11" t="s">
+      <c r="G51" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H51" s="12" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B52" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C52" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="D52" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="E51" s="11" t="s">
+      <c r="E52" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F51" s="11" t="s">
+      <c r="F52" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="G51" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H51" s="11" t="s">
+      <c r="G52" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H52" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="B53" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C52" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D52" s="11" t="s">
+      <c r="C53" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D53" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="E52" s="11" t="s">
+      <c r="E53" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F52" s="11" t="s">
+      <c r="F53" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="G52" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H52" s="11" t="s">
+      <c r="G53" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H53" s="12" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="B54" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C54" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D53" s="11" t="s">
+      <c r="D54" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="E53" s="11" t="s">
+      <c r="E54" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F53" s="11" t="s">
+      <c r="F54" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="G53" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H53" s="11" t="s">
+      <c r="G54" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H54" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B55" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C54" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D54" s="7" t="s">
+      <c r="C55" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D55" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="E54" s="7" t="s">
+      <c r="E55" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="F54" s="7" t="s">
+      <c r="F55" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="G54" s="7" t="s">
+      <c r="G55" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="H54" s="7" t="s">
+      <c r="H55" s="12" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B56" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="C55" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D55" s="7" t="s">
+      <c r="C56" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="E56" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F55" s="7" t="s">
+      <c r="F56" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G55" s="7" t="s">
+      <c r="G56" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="H55" s="7" t="s">
+      <c r="H56" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B57" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C56" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D56" s="7" t="s">
+      <c r="C57" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D57" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="E57" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F56" s="7" t="s">
+      <c r="F57" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G56" s="7" t="s">
+      <c r="G57" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="H56" s="7" t="s">
+      <c r="H57" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B58" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="C57" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D57" s="7" t="s">
+      <c r="C58" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D58" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="E57" s="7" t="s">
+      <c r="E58" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F57" s="7" t="s">
+      <c r="F58" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G57" s="7" t="s">
+      <c r="G58" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="H57" s="7" t="s">
+      <c r="H58" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B59" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="C58" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D58" s="7" t="s">
+      <c r="C59" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D59" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="E58" s="7" t="s">
+      <c r="E59" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F58" s="7" t="s">
+      <c r="F59" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G58" s="7" t="s">
+      <c r="G59" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="H58" s="7" t="s">
+      <c r="H59" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B60" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C59" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D59" s="7" t="s">
+      <c r="C60" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D60" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="E59" s="7" t="s">
+      <c r="E60" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F59" s="7" t="s">
+      <c r="F60" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="G59" s="7" t="s">
+      <c r="G60" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="H59" s="7" t="s">
+      <c r="H60" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B61" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="C60" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D60" s="7" t="s">
+      <c r="C61" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D61" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="E60" s="7" t="s">
+      <c r="E61" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F60" s="7" t="s">
+      <c r="F61" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="G60" s="7" t="s">
+      <c r="G61" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="H60" s="7" t="s">
+      <c r="H61" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B62" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="C61" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D61" s="7" t="s">
+      <c r="C62" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D62" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="E61" s="7" t="s">
+      <c r="E62" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="F61" s="7" t="s">
+      <c r="F62" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="G61" s="7" t="s">
+      <c r="G62" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="H61" s="7" t="s">
+      <c r="H62" s="12" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B63" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="C62" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D62" s="7" t="s">
+      <c r="C63" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D63" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="E62" s="7" t="s">
+      <c r="E63" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="F62" s="7" t="s">
+      <c r="F63" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="G62" s="7" t="s">
+      <c r="G63" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="H62" s="7" t="s">
+      <c r="H63" s="12" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B64" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="C63" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D63" s="7" t="s">
+      <c r="C64" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D64" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="E63" s="7" t="s">
+      <c r="E64" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="F63" s="7" t="s">
+      <c r="F64" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="G63" s="7" t="s">
+      <c r="G64" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="H63" s="7" t="s">
+      <c r="H64" s="12" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B65" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C64" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D64" s="7" t="s">
+      <c r="C65" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D65" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="E64" s="7" t="s">
+      <c r="E65" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="F64" s="7" t="s">
+      <c r="F65" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="G64" s="7" t="s">
+      <c r="G65" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="H64" s="7" t="s">
+      <c r="H65" s="12" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="8" t="s">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B66" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="C65" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D65" s="8" t="s">
+      <c r="C66" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="E65" s="8" t="s">
+      <c r="E66" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F65" s="8" t="s">
+      <c r="F66" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G65" s="8" t="s">
+      <c r="G66" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="H65" s="8" t="s">
+      <c r="H66" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="8" t="s">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B67" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="C66" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D66" s="8" t="s">
+      <c r="C67" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D67" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="E66" s="8" t="s">
+      <c r="E67" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F66" s="8" t="s">
+      <c r="F67" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="G66" s="8" t="s">
+      <c r="G67" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="H66" s="8" t="s">
+      <c r="H67" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="8" t="s">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="B68" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="C67" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D67" s="8" t="s">
+      <c r="C68" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="E67" s="8" t="s">
+      <c r="E68" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F67" s="8" t="s">
+      <c r="F68" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G67" s="8" t="s">
+      <c r="G68" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="H67" s="8" t="s">
+      <c r="H68" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
+    <row r="71" spans="1:11" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-    </row>
-    <row r="72" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A72" s="13" t="s">
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+    </row>
+    <row r="73" spans="1:11" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="A73" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B72" s="14"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="H72" s="17" t="s">
+      <c r="B73" s="17"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="I72" s="17"/>
-      <c r="J72" s="17"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="H73" s="19"/>
+      <c r="I73" s="19"/>
+      <c r="J73" s="19"/>
+      <c r="K73" s="7"/>
+    </row>
+    <row r="74" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A74" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B74" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C74" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D74" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="E74" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F73" s="3" t="s">
+      <c r="F74" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G73" s="19" t="s">
+      <c r="G74" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="H73" s="20"/>
-      <c r="I73" s="20"/>
-      <c r="J73" s="20"/>
-      <c r="K73" s="20"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" s="9" t="s">
+      <c r="H74" s="16"/>
+      <c r="I74" s="16"/>
+      <c r="J74" s="16"/>
+      <c r="K74" s="16"/>
+    </row>
+    <row r="75" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A75" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="B75" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="C75" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D74" s="9" t="s">
+      <c r="D75" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E74" s="9" t="s">
+      <c r="E75" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="F74" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="G74" s="19"/>
-      <c r="H74" s="20"/>
-      <c r="I74" s="20"/>
-      <c r="J74" s="20"/>
-      <c r="K74" s="20"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="9" t="s">
+      <c r="F75" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="G75" s="6"/>
+      <c r="H75" s="7"/>
+      <c r="I75" s="7"/>
+      <c r="J75" s="7"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="B76" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C75" s="9" t="s">
+      <c r="C76" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D75" s="9" t="s">
+      <c r="D76" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E75" s="9" t="s">
+      <c r="E76" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="F75" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="9" t="s">
+      <c r="F76" s="12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="B77" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C76" s="9" t="s">
+      <c r="C77" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D76" s="9" t="s">
+      <c r="D77" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E76" s="9" t="s">
+      <c r="E77" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="F76" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A79" s="15" t="s">
+      <c r="F77" s="12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="A80" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B79" s="15"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+      <c r="B80" s="25"/>
+      <c r="C80" s="25"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="25"/>
+      <c r="F80" s="25"/>
+      <c r="G80" s="25"/>
+      <c r="H80" s="25"/>
+    </row>
+    <row r="81" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A81" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B81" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="C81" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D80" s="3" t="s">
+      <c r="D81" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E80" s="3" t="s">
+      <c r="E81" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F80" s="3" t="s">
+      <c r="F81" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G80" s="3" t="s">
+      <c r="G81" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="H80" s="3" t="s">
+      <c r="H81" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="6" t="s">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="B81" s="6" t="s">
+      <c r="B82" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C81" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D81" s="6" t="s">
+      <c r="C82" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D82" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="E81" s="6" t="s">
+      <c r="E82" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F81" s="6" t="s">
+      <c r="F82" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G81" s="6" t="s">
+      <c r="G82" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="H81" s="6" t="s">
+      <c r="H82" s="12" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="11" t="s">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B82" s="11" t="s">
+      <c r="B83" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="C82" s="11" t="s">
+      <c r="C83" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D82" s="11" t="s">
+      <c r="D83" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="E82" s="11" t="s">
+      <c r="E83" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F82" s="11" t="s">
+      <c r="F83" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="G82" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H82" s="11" t="s">
+      <c r="G83" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H83" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="11" t="s">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B83" s="11" t="s">
+      <c r="B84" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C83" s="11" t="s">
+      <c r="C84" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D83" s="11" t="s">
+      <c r="D84" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="E83" s="11" t="s">
+      <c r="E84" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F83" s="11" t="s">
+      <c r="F84" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="G83" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H83" s="11" t="s">
+      <c r="G84" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H84" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="10" t="s">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B84" s="10" t="s">
+      <c r="B85" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C84" s="10" t="s">
+      <c r="C85" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D84" s="10" t="s">
+      <c r="D85" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="E84" s="10" t="s">
+      <c r="E85" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F84" s="10" t="s">
+      <c r="F85" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G84" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H84" s="10" t="s">
+      <c r="G85" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H85" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="10" t="s">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="B85" s="10" t="s">
+      <c r="B86" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C85" s="10" t="s">
+      <c r="C86" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D85" s="10" t="s">
+      <c r="D86" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="E85" s="10" t="s">
+      <c r="E86" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F85" s="10" t="s">
+      <c r="F86" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G85" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H85" s="10" t="s">
+      <c r="G86" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H86" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="10" t="s">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="B86" s="10" t="s">
+      <c r="B87" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C86" s="10" t="s">
+      <c r="C87" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D86" s="10" t="s">
+      <c r="D87" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="E86" s="10" t="s">
+      <c r="E87" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F86" s="10" t="s">
+      <c r="F87" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G86" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H86" s="10" t="s">
+      <c r="G87" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H87" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="11" t="s">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B87" s="11" t="s">
+      <c r="B88" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C87" s="11" t="s">
+      <c r="C88" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D87" s="11" t="s">
+      <c r="D88" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="E87" s="11" t="s">
+      <c r="E88" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F87" s="11" t="s">
+      <c r="F88" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="G87" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H87" s="11" t="s">
+      <c r="G88" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H88" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="11" t="s">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="B88" s="11" t="s">
+      <c r="B89" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C88" s="11" t="s">
+      <c r="C89" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D88" s="11" t="s">
+      <c r="D89" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="E88" s="11" t="s">
+      <c r="E89" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F88" s="11" t="s">
+      <c r="F89" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="G88" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H88" s="11" t="s">
+      <c r="G89" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H89" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="10" t="s">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="B89" s="10" t="s">
+      <c r="B90" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="C89" s="10" t="s">
+      <c r="C90" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D89" s="10" t="s">
+      <c r="D90" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="E89" s="10" t="s">
+      <c r="E90" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F89" s="10" t="s">
+      <c r="F90" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G89" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H89" s="10" t="s">
+      <c r="G90" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H90" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="10" t="s">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="B90" s="10" t="s">
+      <c r="B91" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C90" s="10" t="s">
+      <c r="C91" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D90" s="10" t="s">
+      <c r="D91" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="E90" s="10" t="s">
+      <c r="E91" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F90" s="10" t="s">
+      <c r="F91" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G90" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H90" s="10" t="s">
+      <c r="G91" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H91" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="10" t="s">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="B91" s="10" t="s">
+      <c r="B92" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="C91" s="10" t="s">
+      <c r="C92" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D91" s="10" t="s">
+      <c r="D92" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="E91" s="10" t="s">
+      <c r="E92" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F91" s="10" t="s">
+      <c r="F92" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G91" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H91" s="10" t="s">
+      <c r="G92" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H92" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="7" t="s">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B92" s="7" t="s">
+      <c r="B93" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C92" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D92" s="7" t="s">
+      <c r="C93" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D93" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="E92" s="7" t="s">
+      <c r="E93" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="F92" s="7" t="s">
+      <c r="F93" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G92" s="7" t="s">
+      <c r="G93" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="H92" s="7" t="s">
+      <c r="H93" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="7" t="s">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B93" s="7" t="s">
+      <c r="B94" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C93" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D93" s="7" t="s">
+      <c r="C94" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D94" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="E93" s="7" t="s">
+      <c r="E94" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F93" s="7" t="s">
+      <c r="F94" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="G93" s="7" t="s">
+      <c r="G94" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="H93" s="7" t="s">
+      <c r="H94" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="7" t="s">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B94" s="7" t="s">
+      <c r="B95" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C94" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D94" s="7" t="s">
+      <c r="C95" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D95" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="E94" s="7" t="s">
+      <c r="E95" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="F94" s="7" t="s">
+      <c r="F95" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G94" s="7" t="s">
+      <c r="G95" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="H94" s="7" t="s">
+      <c r="H95" s="12" t="s">
         <v>181</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A80:H80"/>
+    <mergeCell ref="G73:J73"/>
+    <mergeCell ref="G74:K74"/>
     <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="G5:K6"/>
-    <mergeCell ref="H72:J72"/>
-    <mergeCell ref="G73:K74"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A45:H45"/>
+    <mergeCell ref="A73:F73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>